<commit_message>
ajuste migracion proceso judicial
</commit_message>
<xml_diff>
--- a/migracion/ProcesosJudiciales.xlsx
+++ b/migracion/ProcesosJudiciales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\DesarrolloWeb358\gestion-global\migracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8073061A-E83D-4936-992E-698562BE821C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FB6C14-FBF9-48A6-8EC0-969A2454B514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="CUADRO GENERAL 2025" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CUADRO GENERAL 2025'!$A$1:$H$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CUADRO GENERAL 2025'!$A$1:$H$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>DEMANDADOS</t>
   </si>
@@ -40,122 +40,6 @@
     <t>OBSERVACIONES</t>
   </si>
   <si>
-    <t>NICOLL</t>
-  </si>
-  <si>
-    <t>6-501</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GLORIA ESPERANZA SIERRA Y
-JAIME ENRIQUE ROJAS RUBIO </t>
-  </si>
-  <si>
-    <t>25 PC</t>
-  </si>
-  <si>
-    <t>11001410375120220092800</t>
-  </si>
-  <si>
-    <t>KENNEDY</t>
-  </si>
-  <si>
-    <t>24-02-2025 AL DESPACHO CON SOLICITUD DE SENTENCIA</t>
-  </si>
-  <si>
-    <t>7-101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-GERMAN OSWALDO GONZALEZ GARZON Y GRACIELA DEL PILAR CRUZ GAITAN
-</t>
-  </si>
-  <si>
-    <t>26 PC</t>
-  </si>
-  <si>
-    <t>11001410375220220091100</t>
-  </si>
-  <si>
-    <t>27-05-2025 AUTO RESUELVE SOLICITUD, INFORME GESTION DEL SECUESTRE Y TIENE NOTIFICADO IMPROCEDENTE.</t>
-  </si>
-  <si>
-    <t>30-401</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-MARLIDIS RAMOS BALCAZAR 
-</t>
-  </si>
-  <si>
-    <t>2022-930</t>
-  </si>
-  <si>
-    <t>09-05-2025 SENTENCIA FAVORABLE</t>
-  </si>
-  <si>
-    <t>14 502</t>
-  </si>
-  <si>
-    <t>WILMER FABIAN DELGADO MOLINA Y KAREHN ALEJANDRA MEDINA RODRIGUEZ</t>
-  </si>
-  <si>
-    <t>2022-926</t>
-  </si>
-  <si>
-    <t>04-03-2025 AL DESPACHO. 17-02-2025 SE RADICA 291. 26-02-2025 se solicito expediente , PENDIENTE 292</t>
-  </si>
-  <si>
-    <t>CASA LINDA</t>
-  </si>
-  <si>
-    <t>5-202</t>
-  </si>
-  <si>
-    <t>JOHN JAIDER SANCHEZ ARDILLA Y DIEGO ALONSO RODRIGUEZ BERMUDEZ</t>
-  </si>
-  <si>
-    <t>02 PC</t>
-  </si>
-  <si>
-    <t>25754418900220250082600</t>
-  </si>
-  <si>
-    <t>SOACHA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17/07/2025 se radico demanda 21/07/2025 al despacho 25//07/025 auto inadmite 31/07/2025 se subsana la demanda 04/08/2025 al despacho 06/08/2025 auo libra mandamiento </t>
-  </si>
-  <si>
-    <t>PALO DE ROSA</t>
-  </si>
-  <si>
-    <t>10-503</t>
-  </si>
-  <si>
-    <t>SAIT SUAREZ PEÑA</t>
-  </si>
-  <si>
-    <t>03 PC</t>
-  </si>
-  <si>
-    <t>25754418900320250040200</t>
-  </si>
-  <si>
-    <t>22-04-2025 se volvio a radicar demanda nuevamente 06/05/2025 SE SOLICITO LINK DEL EXPEDIENTE 13/05/2025 correo enviado inofrmando que se encuentra al despacho 22/05/2025 auto inadmite 27/05/2025 se envia memorial de subsanacion. VOLVER A PRESENTAR</t>
-  </si>
-  <si>
-    <t>11-104</t>
-  </si>
-  <si>
-    <t>RUTH YANET LARA TORRES</t>
-  </si>
-  <si>
-    <t>25754418900220250083800</t>
-  </si>
-  <si>
-    <t>30/05/2025 se radico demanda 10/07/2025 auto inadmite 22/07/2025 se radico demanda 31/07/2025 auto inadmite 11/08/2025 se envio memorial de subsanacion</t>
-  </si>
-  <si>
     <t>LAURA</t>
   </si>
   <si>
@@ -166,13 +50,64 @@
   </si>
   <si>
     <t>UBICACION</t>
+  </si>
+  <si>
+    <t>F-103</t>
+  </si>
+  <si>
+    <t>ALEX MILLER GOMEZ GONZALEZ Y AMPARO PALACIO NIETO</t>
+  </si>
+  <si>
+    <t>76 CM</t>
+  </si>
+  <si>
+    <t>11001400307620210078100</t>
+  </si>
+  <si>
+    <t>CENTRO</t>
+  </si>
+  <si>
+    <t>06-06-2025 AL DESPACHO CON LIQUIDACION DEL CREDITO</t>
+  </si>
+  <si>
+    <t>G-102</t>
+  </si>
+  <si>
+    <t>BERNANDO DAVID MATORRELLA BATISTA</t>
+  </si>
+  <si>
+    <t>05 PC</t>
+  </si>
+  <si>
+    <t>2024-046</t>
+  </si>
+  <si>
+    <t>FONTIBON</t>
+  </si>
+  <si>
+    <t>10-04-2025 SE SOLICITO LINK DEL EXPEDIENTE PERO ENVIARON FUE 2023-46 TOCA VOLVER A SOLICITARLO</t>
+  </si>
+  <si>
+    <t>F-801</t>
+  </si>
+  <si>
+    <t>JORGE ANDRES MARTINEZ GALVIS</t>
+  </si>
+  <si>
+    <t>2024-043</t>
+  </si>
+  <si>
+    <t>10-04-2025 SE SOLICITO LINK DEL EXPEDIENTE. OK. 03-12-2024 OFICIO 1646 DE EMBARGO BANCOS Y 1647 INSTRUMENTOS PUBLICOS./31-01-2024 CON MANDAMIENTO Y MEDICAS CAUTERALES.</t>
+  </si>
+  <si>
+    <t>FECHA DE ULTIMA REVISION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,11 +138,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -228,12 +158,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEAD1DC"/>
-        <bgColor rgb="FFEAD1DC"/>
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -256,22 +186,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -288,47 +207,38 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -659,11 +569,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -676,17 +586,18 @@
     <col min="6" max="6" width="20.453125" customWidth="1"/>
     <col min="7" max="7" width="10.90625" customWidth="1"/>
     <col min="8" max="8" width="55" customWidth="1"/>
+    <col min="9" max="9" width="22.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -703,251 +614,167 @@
       <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="I1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6">
-        <v>901268833</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="B2" s="11">
+        <v>900334680</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="D2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="E2" s="12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="69" x14ac:dyDescent="0.35">
+      <c r="F2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="16">
+        <v>45866</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6">
-        <v>901268833</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="B3" s="11">
+        <v>900334680</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="10" t="s">
+      <c r="D3" s="13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="E3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="16">
+        <v>45845</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6">
-        <v>901268833</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="11">
+        <v>900334680</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="F4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="6">
-        <v>901268833</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="10" t="s">
+      <c r="H4" s="15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="35.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="46" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="19"/>
-    </row>
-    <row r="10" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="19"/>
-    </row>
-    <row r="11" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="19"/>
-    </row>
-    <row r="12" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="19"/>
-    </row>
-    <row r="13" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="16"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="19"/>
-    </row>
-    <row r="14" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="16"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="19"/>
+      <c r="I4" s="16">
+        <v>45845</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H8" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H4" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <dataValidations count="2">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:I4" xr:uid="{94E2583E-2C32-47D5-81C8-F1B96A86DDE8}">
+      <formula1>OR(NOT(ISERROR(DATEVALUE(I2))), AND(ISNUMBER(I2), LEFT(CELL("format", I2))="D"))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="G2:G4" xr:uid="{336437C5-6D1A-4FB5-B8E7-F4EB3B14BC90}">
+      <formula1>"KENNEDY,SOACHA,BOSA,EJECUCION,CENTRO,PUENTE ARANDA,USAQUEN,FONTIBON,SAN CRISTOBAL,MADRID,C.BOLIVAR,CARMEN DEAPICALA,SUBA"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="5" pageOrder="overThenDown" orientation="landscape"/>
 </worksheet>

</xml_diff>